<commit_message>
add write to patientlist class
</commit_message>
<xml_diff>
--- a/Patient_List.xlsx
+++ b/Patient_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="24">
   <si>
     <t>Patient ID</t>
   </si>
@@ -83,12 +83,16 @@
   </si>
   <si>
     <t>charlie.white@example.com</t>
+  </si>
+  <si>
+    <t>Appointment notes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -440,7 +444,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:H4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -465,6 +469,9 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">

</xml_diff>

<commit_message>
changed to maven project(do in hospital_management_system)
</commit_message>
<xml_diff>
--- a/Patient_List.xlsx
+++ b/Patient_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
   <si>
     <t>Patient ID</t>
   </si>
@@ -490,73 +490,73 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" t="s" s="0">
         <v>27</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" t="s">
+      <c r="A2" t="s" s="0">
         <v>6</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" t="s" s="0">
         <v>9</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" t="s" s="0">
         <v>12</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" t="s" s="0">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" t="s" s="0">
         <v>17</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" t="s" s="0">
         <v>20</v>
       </c>
-      <c r="H2" t="s">
+      <c r="H2" t="s" s="0">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" t="s">
+      <c r="A3" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" t="s" s="0">
         <v>10</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" t="s" s="0">
         <v>13</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" t="s" s="0">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" t="s" s="0">
         <v>21</v>
       </c>
-      <c r="H3" t="s">
-        <v>30</v>
+      <c r="H3" t="s" s="0">
+        <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" t="s">
+      <c r="A4" t="s" s="0">
         <v>8</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" t="s" s="0">
         <v>11</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" t="s" s="0">
         <v>14</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" t="s" s="0">
         <v>16</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" t="s" s="0">
         <v>19</v>
       </c>
-      <c r="F4" t="s">
+      <c r="F4" t="s" s="0">
         <v>22</v>
       </c>
     </row>

</xml_diff>

<commit_message>
cahnged read write method
</commit_message>
<xml_diff>
--- a/Patient_List.xlsx
+++ b/Patient_List.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Patient ID</t>
   </si>
@@ -107,6 +107,9 @@
   </si>
   <si>
     <t>lol</t>
+  </si>
+  <si>
+    <t>cocksmal</t>
   </si>
 </sst>
 </file>
@@ -537,7 +540,7 @@
         <v>21</v>
       </c>
       <c r="H3" t="s" s="0">
-        <v>26</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:6">

</xml_diff>